<commit_message>
HW: Update LNA + Diff probe with latest version
</commit_message>
<xml_diff>
--- a/hardware/tools/lna_3v/lna3v_eagleproj/bom_lnasimple.xlsx
+++ b/hardware/tools/lna_3v/lna3v_eagleproj/bom_lnasimple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Line No.</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Package</t>
   </si>
   <si>
-    <t>Digikey</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -123,42 +120,15 @@
     <t>220R</t>
   </si>
   <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>APT2012YC</t>
-  </si>
-  <si>
-    <t>754-1135-1-ND</t>
-  </si>
-  <si>
-    <t>Kingbright</t>
-  </si>
-  <si>
-    <t>WM2711-ND</t>
-  </si>
-  <si>
-    <t>Molex Inc</t>
-  </si>
-  <si>
-    <t>Tol</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
     <t>Vendor</t>
   </si>
   <si>
-    <t>Example Part No.</t>
-  </si>
-  <si>
     <t>Sub Type</t>
   </si>
   <si>
-    <t>ANY</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -171,10 +141,55 @@
     <t>6-pin male, shrouded</t>
   </si>
   <si>
-    <t>Mount Backside</t>
-  </si>
-  <si>
     <t>SMA Female, 1.6mm edge PCB</t>
+  </si>
+  <si>
+    <t>Part No</t>
+  </si>
+  <si>
+    <t>Digikey Part No</t>
+  </si>
+  <si>
+    <t>Newark Part No</t>
+  </si>
+  <si>
+    <t>P221HCT-ND</t>
+  </si>
+  <si>
+    <t>GENERIC</t>
+  </si>
+  <si>
+    <t>75869-131LF</t>
+  </si>
+  <si>
+    <t>FCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 62K8134</t>
+  </si>
+  <si>
+    <t>609-2845-ND</t>
+  </si>
+  <si>
+    <t>Will be provided - do not order</t>
+  </si>
+  <si>
+    <t>Mounts Backside</t>
+  </si>
+  <si>
+    <t>73251-1150</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>LTST-C194KRKT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">160-1835-1-ND </t>
+  </si>
+  <si>
+    <t>Red LED</t>
   </si>
 </sst>
 </file>
@@ -198,15 +213,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -214,26 +241,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,299 +591,407 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>41</v>
+      <c r="F1" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="I7" s="4"/>
+      <c r="J7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="B10" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="D10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>